<commit_message>
add effort form from Bruce and include in compiled effort spreadsheet
</commit_message>
<xml_diff>
--- a/data/compiling/2024/CRCA/effort/CBC_Cacao_2024_effort_compiled.xlsx
+++ b/data/compiling/2024/CRCA/effort/CBC_Cacao_2024_effort_compiled.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francisjoyce/GitHub/ACG-CBC-data/data/compiling/2024/CRCA/effort/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E1CDEA-6E8E-7E40-B146-A9A1A23A6832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42C1ED9-4462-F84E-A844-0E9AAD9544C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2000" yWindow="500" windowWidth="24100" windowHeight="17440" xr2:uid="{0295E492-2659-ED4A-BD93-CE46759B4404}"/>
+    <workbookView xWindow="16780" yWindow="2240" windowWidth="24100" windowHeight="17440" xr2:uid="{0295E492-2659-ED4A-BD93-CE46759B4404}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
   <si>
     <t>Nombre de ruta</t>
   </si>
@@ -173,26 +173,35 @@
     <t>Estuvimos aprovechando la infrastructura del Restaurante de Nueva Zelandia y el Galerón de San Gerardo, además del carro, para no mojarnos demasiado y no mojar el equipo óptico. Un dia muy lluvioso per cada vez que paró la lluvia aprovechamos los minutos!</t>
   </si>
   <si>
-    <t>Freddy Quesada</t>
+    <t>suroeste</t>
+  </si>
+  <si>
+    <t>nublado total, con neblina</t>
+  </si>
+  <si>
+    <t>leve</t>
+  </si>
+  <si>
+    <t>Compiled (total)</t>
+  </si>
+  <si>
+    <t>leve, lluvia, seco</t>
+  </si>
+  <si>
+    <t>Freddy Quesada, Amanda Young, Nelson Espinoza Mora, Erick Picado Zeledón</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -214,6 +223,28 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -234,21 +265,23 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -584,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3E85EDE-13B4-7449-81E7-124D4DE6EFA2}">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Z6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -617,83 +650,83 @@
     <col min="26" max="26" width="31.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="8" t="s">
         <v>23</v>
       </c>
     </row>
@@ -704,11 +737,74 @@
       <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.23541666666666666</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0.67152777777777772</v>
+      </c>
+      <c r="H2">
+        <v>17</v>
+      </c>
+      <c r="I2">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
         <v>45</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>15</v>
+      </c>
+      <c r="M2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q2">
+        <v>11</v>
+      </c>
+      <c r="R2">
+        <v>10.5</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0.2</v>
+      </c>
+      <c r="X2">
+        <v>0.5</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
@@ -727,10 +823,10 @@
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>0.3840277777777778</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>0.50277777777777777</v>
       </c>
       <c r="Q3">
@@ -756,7 +852,7 @@
       <c r="B4" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D4" t="s">
@@ -765,10 +861,10 @@
       <c r="E4">
         <v>2</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>0.41666666666666669</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>0.6875</v>
       </c>
       <c r="H4">
@@ -827,19 +923,19 @@
       <c r="B5" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>41</v>
       </c>
       <c r="E5">
         <v>11</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>0.29166666666666669</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>0.64583333333333337</v>
       </c>
       <c r="H5">
@@ -890,8 +986,83 @@
       <c r="Y5">
         <v>0</v>
       </c>
-      <c r="Z5" s="7" t="s">
+      <c r="Z5" s="6" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6">
+        <f>SUM(E2:E5)</f>
+        <v>19</v>
+      </c>
+      <c r="F6" s="2">
+        <f>MIN(F2:F5)</f>
+        <v>0.23541666666666666</v>
+      </c>
+      <c r="G6" s="4">
+        <f>MAX(G2:G5)</f>
+        <v>0.6875</v>
+      </c>
+      <c r="H6">
+        <f>MIN(H2:H5)</f>
+        <v>17</v>
+      </c>
+      <c r="I6">
+        <f>MAX(I2:I5)</f>
+        <v>32</v>
+      </c>
+      <c r="J6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6">
+        <f>MIN(K2:K5)</f>
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <f>MAX(L2:L5)</f>
+        <v>35</v>
+      </c>
+      <c r="M6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N6" t="s">
+        <v>49</v>
+      </c>
+      <c r="O6" t="s">
+        <v>46</v>
+      </c>
+      <c r="P6" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q6">
+        <f>SUM(Q2:Q5)</f>
+        <v>14.48</v>
+      </c>
+      <c r="R6">
+        <f>SUM(R2:R5)</f>
+        <v>13.85</v>
+      </c>
+      <c r="S6">
+        <f>SUM(S2:S5)</f>
+        <v>37</v>
+      </c>
+      <c r="T6">
+        <f>SUM(T2:T5)</f>
+        <v>14</v>
+      </c>
+      <c r="W6">
+        <f>SUM(W2:W5)</f>
+        <v>0.2</v>
+      </c>
+      <c r="X6">
+        <f>SUM(X2:X5)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>